<commit_message>
Modified RöntgenNormal.xlsx, added "Aorta ascendens" & "Aorta descendens" synonyms, added "Zweiter Shaldon-Katheter" synonym
</commit_message>
<xml_diff>
--- a/Schablonen/RöntgenNormal.xlsx
+++ b/Schablonen/RöntgenNormal.xlsx
@@ -267,7 +267,7 @@
     <t>2. Shaldon-Katheter</t>
   </si>
   <si>
-    <t>2. Shaldon-Katheter;weiterer Shaldon;weiterer Shaldon Katheter;zweiter Shaldon Katheter;zweiter Shaldon;2. Shaldon</t>
+    <t>2. Shaldon-Katheter;weiterer Shaldon;weiterer Shaldon Katheter;zweiter Shaldon Katheter;zweiter Shaldon-Katheter;zweiter Shaldon;2. Shaldon</t>
   </si>
   <si>
     <t>I10</t>
@@ -816,7 +816,7 @@
     <t>Aorta asc. / Aorta desc.</t>
   </si>
   <si>
-    <t>asc/desc</t>
+    <t>asc;Aorta ascendens/desc;Aorta descendens</t>
   </si>
   <si>
     <t>im Bereich der ...</t>
@@ -1423,6 +1423,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -1431,9 +1434,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -2281,7 +2281,7 @@
       <c r="C22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E22" s="1"/>
@@ -2599,10 +2599,10 @@
       <c r="K33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="L33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M33" s="2"/>
+      <c r="M33" s="3"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1" t="s">
         <v>110</v>
@@ -2629,10 +2629,10 @@
       <c r="K34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="L34" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M34" s="2"/>
+      <c r="M34" s="3"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1" t="s">
         <v>113</v>
@@ -2686,13 +2686,13 @@
       <c r="J36" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="K36" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="L36" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M36" s="2"/>
+      <c r="M36" s="3"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1" t="s">
         <v>121</v>
@@ -2838,8 +2838,8 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -2864,15 +2864,15 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="K43" s="5" t="s">
         <v>141</v>
       </c>
       <c r="L43" s="1" t="s">
@@ -2915,7 +2915,7 @@
       <c r="C45" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="2" t="s">
         <v>148</v>
       </c>
       <c r="E45" s="1"/>
@@ -3098,7 +3098,7 @@
       <c r="J51" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="K51" s="3" t="s">
         <v>177</v>
       </c>
       <c r="L51" s="1" t="s">
@@ -3156,7 +3156,7 @@
       <c r="J53" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="K53" s="3" t="s">
         <v>177</v>
       </c>
       <c r="L53" s="1" t="s">
@@ -3184,7 +3184,7 @@
       <c r="J54" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="K54" s="3" t="s">
         <v>182</v>
       </c>
       <c r="L54" s="1" t="s">
@@ -3214,7 +3214,7 @@
       <c r="J55" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="K55" s="2" t="s">
+      <c r="K55" s="3" t="s">
         <v>177</v>
       </c>
       <c r="L55" s="1" t="s">
@@ -3242,7 +3242,7 @@
       <c r="J56" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="K56" s="2" t="s">
+      <c r="K56" s="3" t="s">
         <v>182</v>
       </c>
       <c r="L56" s="1" t="s">
@@ -3815,7 +3815,7 @@
       <c r="K76" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="L76" s="1" t="s">
+      <c r="L76" s="2" t="s">
         <v>266</v>
       </c>
       <c r="M76" s="1"/>

</xml_diff>

<commit_message>
Modified RöntgenNormal.xlsx, added "Herz Thoraxquotient" synonym, added "freie abdominale Luft" synonym, added "WT-Emphysem" synonym
</commit_message>
<xml_diff>
--- a/Schablonen/RöntgenNormal.xlsx
+++ b/Schablonen/RöntgenNormal.xlsx
@@ -231,7 +231,7 @@
     <t>2. ZVK</t>
   </si>
   <si>
-    <t>2. ZVK;weiterer ZVK;zweiter ZVK</t>
+    <t>2. ZVK;weiterer ZVK;zweiter ZVK;zweites ZVK</t>
   </si>
   <si>
     <t>I4</t>
@@ -876,7 +876,7 @@
     <t>Herz-Thorax-Quotient</t>
   </si>
   <si>
-    <t>Herz Thorax Quotient;HTQ;HT Quotient;Herz-Thorax-Quotient</t>
+    <t>Herz Thorax Quotient;HTQ;HT Quotient;Herz-Thorax-Quotient;Herz Thoraxquotient</t>
   </si>
   <si>
     <t>H1</t>
@@ -1203,7 +1203,7 @@
     <t>FAL</t>
   </si>
   <si>
-    <t>FAL;freie abdominelle Luft</t>
+    <t>FAL;freie abdominelle Luft;freie abdominale Luft</t>
   </si>
   <si>
     <t>O1</t>
@@ -1227,7 +1227,7 @@
     <t>WT normal</t>
   </si>
   <si>
-    <t>WT normal;Weichteile normal</t>
+    <t>WT normal;Weichteile normal;WT-normal</t>
   </si>
   <si>
     <t>WT-Emphysem,weiteres WT-Emphysem</t>
@@ -1239,7 +1239,7 @@
     <t>WT-Emphysem</t>
   </si>
   <si>
-    <t>Weichteil Emphysem;WT Emphysem;Weichteileemphysem;Weichteilemphysem</t>
+    <t>Weichteil Emphysem;WT Emphysem;Weichteileemphysem;Weichteilemphysem;Weichteil-Emphysem;WT-Emphysem</t>
   </si>
   <si>
     <t>W1</t>
@@ -1260,7 +1260,7 @@
     <t>weiteres WT-Emphysem</t>
   </si>
   <si>
-    <t>weiteres Weichteil Emphysem;weiteres WT Emphysem;weiteres Weichteileemphysem;weiteres Weichteilemphysem</t>
+    <t>weiteres Weichteil Emphysem;weiteres WT Emphysem;weiteres Weichteileemphysem;weiteres Weichteilemphysem;weiteres WT-Emphysem</t>
   </si>
   <si>
     <t>W4</t>
@@ -2121,7 +2121,7 @@
       <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="1"/>
@@ -3969,7 +3969,7 @@
       <c r="C82" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" s="2" t="s">
         <v>286</v>
       </c>
       <c r="E82" s="1"/>
@@ -4845,7 +4845,7 @@
       <c r="C114" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D114" s="2" t="s">
         <v>395</v>
       </c>
       <c r="E114" s="1"/>
@@ -4905,7 +4905,7 @@
       <c r="C116" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" s="2" t="s">
         <v>403</v>
       </c>
       <c r="E116" s="1" t="s">
@@ -4933,7 +4933,7 @@
       <c r="C117" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D117" s="2" t="s">
         <v>407</v>
       </c>
       <c r="E117" s="1"/>
@@ -5015,7 +5015,7 @@
       <c r="C120" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D120" s="2" t="s">
         <v>414</v>
       </c>
       <c r="E120" s="1"/>

</xml_diff>